<commit_message>
[IMP] Update import guest
</commit_message>
<xml_diff>
--- a/public/sample_guest_excel.xlsx
+++ b/public/sample_guest_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguonchhay/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguonchhay/projects/laravel/local.wedding.host/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -173,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,6 +187,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -486,10 +489,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>15</v>
@@ -514,10 +517,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -530,14 +533,14 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -548,6 +551,9 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>